<commit_message>
Adding NO_FISH for Sandpiper in NW Appledore in 2016, Byrnes lab
</commit_message>
<xml_diff>
--- a/raw_data/KEEN ONE/Byrnes/2016/NW Appledore 2016/NWAppledore_fish_2016.xlsx
+++ b/raw_data/KEEN ONE/Byrnes/2016/NW Appledore 2016/NWAppledore_fish_2016.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="32200" yWindow="-10820" windowWidth="30140" windowHeight="14780"/>
+    <workbookView xWindow="6580" yWindow="0" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Data Entry" sheetId="1" r:id="rId1"/>
@@ -197,7 +197,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="148">
   <si>
     <t>YEAR</t>
   </si>
@@ -638,6 +638,9 @@
   </si>
   <si>
     <t>NN</t>
+  </si>
+  <si>
+    <t>NO_FISH</t>
   </si>
 </sst>
 </file>
@@ -729,8 +732,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="75">
+  <cellStyleXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -863,7 +868,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="75">
+  <cellStyles count="77">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -901,6 +906,7 @@
     <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -938,6 +944,7 @@
     <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1282,11 +1289,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W7064"/>
+  <dimension ref="A1:W7065"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R36" sqref="R36"/>
+      <selection pane="bottomLeft" activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -2241,7 +2248,10 @@
         <v>142</v>
       </c>
       <c r="G21" t="s">
-        <v>104</v>
+        <v>147</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
       </c>
       <c r="O21" s="25">
         <v>9.4</v>
@@ -2282,31 +2292,22 @@
         <v>141</v>
       </c>
       <c r="F22" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G22" t="s">
-        <v>78</v>
-      </c>
-      <c r="H22">
+        <v>104</v>
+      </c>
+      <c r="O22" s="25">
+        <v>9.4</v>
+      </c>
+      <c r="P22">
+        <v>10.4</v>
+      </c>
+      <c r="Q22">
         <v>3</v>
       </c>
-      <c r="I22" s="9">
-        <v>3</v>
-      </c>
-      <c r="M22">
-        <v>6</v>
-      </c>
-      <c r="O22" s="25">
-        <v>7.4</v>
-      </c>
-      <c r="P22">
-        <v>7.9</v>
-      </c>
-      <c r="Q22">
-        <v>4</v>
-      </c>
       <c r="R22" s="9">
-        <v>11.7</v>
+        <v>12.8</v>
       </c>
       <c r="S22" t="s">
         <v>139</v>
@@ -2338,7 +2339,16 @@
         <v>144</v>
       </c>
       <c r="G23" t="s">
-        <v>81</v>
+        <v>78</v>
+      </c>
+      <c r="H23">
+        <v>3</v>
+      </c>
+      <c r="I23" s="9">
+        <v>3</v>
+      </c>
+      <c r="M23">
+        <v>6</v>
       </c>
       <c r="O23" s="25">
         <v>7.4</v>
@@ -2382,7 +2392,7 @@
         <v>144</v>
       </c>
       <c r="G24" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="O24" s="25">
         <v>7.4</v>
@@ -2426,7 +2436,7 @@
         <v>144</v>
       </c>
       <c r="G25" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="O25" s="25">
         <v>7.4</v>
@@ -2470,7 +2480,7 @@
         <v>144</v>
       </c>
       <c r="G26" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="O26" s="25">
         <v>7.4</v>
@@ -2514,7 +2524,7 @@
         <v>144</v>
       </c>
       <c r="G27" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="O27" s="25">
         <v>7.4</v>
@@ -2558,7 +2568,7 @@
         <v>144</v>
       </c>
       <c r="G28" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="O28" s="25">
         <v>7.4</v>
@@ -2602,7 +2612,7 @@
         <v>144</v>
       </c>
       <c r="G29" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="O29" s="25">
         <v>7.4</v>
@@ -2646,7 +2656,7 @@
         <v>144</v>
       </c>
       <c r="G30" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="O30" s="25">
         <v>7.4</v>
@@ -2690,7 +2700,7 @@
         <v>144</v>
       </c>
       <c r="G31" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="O31" s="25">
         <v>7.4</v>
@@ -2722,43 +2732,34 @@
         <v>8</v>
       </c>
       <c r="C32" s="15">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D32" s="24">
-        <v>42593</v>
+        <v>42591</v>
       </c>
       <c r="E32" t="s">
         <v>141</v>
       </c>
       <c r="F32" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="G32" t="s">
-        <v>78</v>
-      </c>
-      <c r="I32">
+        <v>104</v>
+      </c>
+      <c r="O32" s="25">
+        <v>7.4</v>
+      </c>
+      <c r="P32">
+        <v>7.9</v>
+      </c>
+      <c r="Q32">
         <v>4</v>
       </c>
-      <c r="J32">
-        <v>2</v>
-      </c>
-      <c r="M32">
-        <v>6</v>
-      </c>
-      <c r="O32">
-        <v>9.1</v>
-      </c>
-      <c r="P32">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="Q32">
-        <v>1</v>
-      </c>
       <c r="R32" s="9">
-        <v>15</v>
+        <v>11.7</v>
       </c>
       <c r="S32" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="U32" t="s">
         <v>140</v>
@@ -2787,7 +2788,16 @@
         <v>143</v>
       </c>
       <c r="G33" t="s">
-        <v>81</v>
+        <v>78</v>
+      </c>
+      <c r="I33">
+        <v>4</v>
+      </c>
+      <c r="J33">
+        <v>2</v>
+      </c>
+      <c r="M33">
+        <v>6</v>
       </c>
       <c r="O33">
         <v>9.1</v>
@@ -2831,7 +2841,7 @@
         <v>143</v>
       </c>
       <c r="G34" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="O34">
         <v>9.1</v>
@@ -2875,7 +2885,7 @@
         <v>143</v>
       </c>
       <c r="G35" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="O35">
         <v>9.1</v>
@@ -2919,7 +2929,7 @@
         <v>143</v>
       </c>
       <c r="G36" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="O36">
         <v>9.1</v>
@@ -2963,7 +2973,7 @@
         <v>143</v>
       </c>
       <c r="G37" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="O37">
         <v>9.1</v>
@@ -3007,7 +3017,7 @@
         <v>143</v>
       </c>
       <c r="G38" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="O38">
         <v>9.1</v>
@@ -3051,7 +3061,7 @@
         <v>143</v>
       </c>
       <c r="G39" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="O39">
         <v>9.1</v>
@@ -3095,7 +3105,7 @@
         <v>143</v>
       </c>
       <c r="G40" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="O40">
         <v>9.1</v>
@@ -3139,7 +3149,7 @@
         <v>143</v>
       </c>
       <c r="G41" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="O41">
         <v>9.1</v>
@@ -3163,280 +3173,324 @@
         <v>140</v>
       </c>
     </row>
-    <row r="7011" spans="23:23">
-      <c r="W7011" t="s">
+    <row r="42" spans="1:22">
+      <c r="A42">
+        <v>2016</v>
+      </c>
+      <c r="B42" s="9">
+        <v>8</v>
+      </c>
+      <c r="C42" s="15">
+        <v>11</v>
+      </c>
+      <c r="D42" s="24">
+        <v>42593</v>
+      </c>
+      <c r="E42" t="s">
+        <v>141</v>
+      </c>
+      <c r="F42" t="s">
+        <v>143</v>
+      </c>
+      <c r="G42" t="s">
+        <v>104</v>
+      </c>
+      <c r="O42">
+        <v>9.1</v>
+      </c>
+      <c r="P42">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="Q42">
+        <v>1</v>
+      </c>
+      <c r="R42" s="9">
+        <v>15</v>
+      </c>
+      <c r="S42" t="s">
+        <v>146</v>
+      </c>
+      <c r="U42" t="s">
+        <v>140</v>
+      </c>
+      <c r="V42" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="7012" spans="23:23">
+      <c r="W7012" t="s">
         <v>60</v>
-      </c>
-    </row>
-    <row r="7012" spans="23:23">
-      <c r="W7012" s="11" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="7013" spans="23:23">
       <c r="W7013" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7014" spans="23:23">
       <c r="W7014" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7015" spans="23:23">
       <c r="W7015" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7016" spans="23:23">
       <c r="W7016" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7017" spans="23:23">
       <c r="W7017" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7018" spans="23:23">
+      <c r="W7018" s="11" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7018" spans="23:23">
-      <c r="W7018" s="12" t="s">
+    <row r="7019" spans="23:23">
+      <c r="W7019" s="12" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="7019" spans="23:23">
-      <c r="W7019" s="11" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="7020" spans="23:23">
       <c r="W7020" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7021" spans="23:23">
       <c r="W7021" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7022" spans="23:23">
       <c r="W7022" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7023" spans="23:23">
       <c r="W7023" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7024" spans="23:23">
       <c r="W7024" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7025" spans="23:23">
       <c r="W7025" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7026" spans="23:23">
       <c r="W7026" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7027" spans="23:23">
       <c r="W7027" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7028" spans="23:23">
       <c r="W7028" s="11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7029" spans="23:23">
+      <c r="W7029" s="11" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7029" spans="23:23">
-      <c r="W7029" s="12" t="s">
+    <row r="7030" spans="23:23">
+      <c r="W7030" s="12" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="7030" spans="23:23">
-      <c r="W7030" s="11" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="7031" spans="23:23">
       <c r="W7031" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7032" spans="23:23">
       <c r="W7032" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7033" spans="23:23">
       <c r="W7033" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7034" spans="23:23">
       <c r="W7034" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7035" spans="23:23">
       <c r="W7035" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7036" spans="23:23">
       <c r="W7036" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7037" spans="23:23">
       <c r="W7037" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7038" spans="23:23">
       <c r="W7038" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7039" spans="23:23">
       <c r="W7039" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7040" spans="23:23">
       <c r="W7040" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7041" spans="23:23">
       <c r="W7041" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7042" spans="23:23">
+      <c r="W7042" s="11" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7042" spans="23:23">
-      <c r="W7042" s="12" t="s">
+    <row r="7043" spans="23:23">
+      <c r="W7043" s="12" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="7043" spans="23:23">
-      <c r="W7043" s="11" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="7044" spans="23:23">
       <c r="W7044" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7045" spans="23:23">
       <c r="W7045" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7046" spans="23:23">
       <c r="W7046" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7047" spans="23:23">
       <c r="W7047" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7048" spans="23:23">
       <c r="W7048" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7049" spans="23:23">
       <c r="W7049" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7050" spans="23:23">
       <c r="W7050" s="11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7051" spans="23:23">
+      <c r="W7051" s="11" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="7051" spans="23:23">
-      <c r="W7051" s="12" t="s">
+    <row r="7052" spans="23:23">
+      <c r="W7052" s="12" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="7052" spans="23:23">
-      <c r="W7052" s="11" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="7053" spans="23:23">
       <c r="W7053" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7054" spans="23:23">
       <c r="W7054" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7055" spans="23:23">
+      <c r="W7055" s="11" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="7055" spans="23:23">
-      <c r="W7055" s="12" t="s">
+    <row r="7056" spans="23:23">
+      <c r="W7056" s="12" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="7056" spans="23:23">
-      <c r="W7056" s="11" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="7057" spans="23:23">
       <c r="W7057" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7058" spans="23:23">
       <c r="W7058" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7059" spans="23:23">
       <c r="W7059" s="11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7060" spans="23:23">
+      <c r="W7060" s="11" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="7060" spans="23:23">
-      <c r="W7060" s="13" t="s">
+    <row r="7061" spans="23:23">
+      <c r="W7061" s="13" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="7061" spans="23:23">
-      <c r="W7061" s="11" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="7062" spans="23:23">
       <c r="W7062" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7063" spans="23:23">
       <c r="W7063" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7064" spans="23:23">
       <c r="W7064" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7065" spans="23:23">
+      <c r="W7065" s="11" t="s">
         <v>59</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F11 F42:F1048576">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F11 F43:F1048576">
       <formula1>1</formula1>
       <formula2>8</formula2>
     </dataValidation>
@@ -3455,13 +3509,13 @@
           <x14:formula1>
             <xm:f>'Allowed Codes'!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>G1:G31 G42:G1048576</xm:sqref>
+          <xm:sqref>G43:G1048576 G1:G32</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'[1]Allowed Codes'!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>G32:G41</xm:sqref>
+          <xm:sqref>G33:G42</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>